<commit_message>
easy frontend code refCTORİNG
</commit_message>
<xml_diff>
--- a/tunbis/tunbis/computer_info.xlsx
+++ b/tunbis/tunbis/computer_info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Computer Name</t>
   </si>
@@ -140,40 +140,37 @@
     <t>PolNet</t>
   </si>
   <si>
-    <t>TNC1MRKBTE03</t>
-  </si>
-  <si>
-    <t>Dell Inc.</t>
-  </si>
-  <si>
-    <t>OptiPlex SFF 7020</t>
-  </si>
-  <si>
-    <t>810J374</t>
-  </si>
-  <si>
-    <t>Intel(R) Core(TM) i5-14500</t>
-  </si>
-  <si>
-    <t>Intel(R) UHD Graphics 770</t>
-  </si>
-  <si>
-    <t>1.12.0</t>
-  </si>
-  <si>
-    <t>0CXR46</t>
-  </si>
-  <si>
-    <t>/810J374/CNFCW004A701FF/</t>
-  </si>
-  <si>
-    <t>10.62.112.61</t>
-  </si>
-  <si>
-    <t>2400A NVMe Micron 512GB</t>
-  </si>
-  <si>
-    <t>80CE000080CE</t>
+    <t>TNC1PRTASY10</t>
+  </si>
+  <si>
+    <t>LENOVO</t>
+  </si>
+  <si>
+    <t>10MLS2BX00</t>
+  </si>
+  <si>
+    <t>PC0P5RF7</t>
+  </si>
+  <si>
+    <t>Intel(R) Core(TM) i5-7500 CPU @ 3.40GHz</t>
+  </si>
+  <si>
+    <t>Intel(R) HD Graphics 630</t>
+  </si>
+  <si>
+    <t>M1AKT59A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    </t>
+  </si>
+  <si>
+    <t>10.62.78.185</t>
+  </si>
+  <si>
+    <t>WDC WD5000AZLX-08K2TA0</t>
+  </si>
+  <si>
+    <t>Samsung</t>
   </si>
 </sst>
 </file>
@@ -530,7 +527,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+      <selection activeCell="H2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +656,7 @@
         <v>42</v>
       </c>
       <c r="H2" s="1">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
@@ -670,23 +667,26 @@
       <c r="K2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="1">
+        <v>3106</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1">
+        <v>8</v>
+      </c>
+      <c r="P2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O2" s="1">
-        <v>16</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>48</v>
+      <c r="S2" s="1">
+        <v>465.76</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>31</v>
@@ -710,19 +710,22 @@
         <v>20230623</v>
       </c>
       <c r="AA2" s="1">
-        <v>13.14</v>
+        <v>9.39</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AC2" s="1">
-        <v>5600</v>
+        <v>2400</v>
       </c>
       <c r="AD2" s="1">
         <v>0</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>